<commit_message>
2020-07-03 19:35 1. Moddify report_last_007_days_walk.Rmd 2. Added last two days walks to  data/walks.Rmd 3. Modified functions /    compute_coefficient_of variation.R 4. Modified functions /get_day_roures.R 5. Added functions / report_summary.R
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="106">
   <si>
     <t>walked</t>
   </si>
@@ -341,13 +341,7 @@
     <t>Widespread Dust</t>
   </si>
   <si>
-    <t>6/202020 12:18</t>
-  </si>
-  <si>
-    <t>bAD</t>
-  </si>
-  <si>
-    <t>1`</t>
+    <t>SSW</t>
   </si>
 </sst>
 </file>
@@ -1187,12 +1181,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY133"/>
+  <dimension ref="A1:AY136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K133" sqref="K133"/>
+      <selection pane="bottomLeft" activeCell="AU137" sqref="AU137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11444,7 +11438,7 @@
         <v>2.1333333333333333</v>
       </c>
       <c r="V110" s="1">
-        <f t="shared" ref="V110:V133" si="85">U110-T110</f>
+        <f t="shared" ref="V110:V136" si="85">U110-T110</f>
         <v>3.3333333333333215E-2</v>
       </c>
       <c r="W110" s="1">
@@ -14593,8 +14587,8 @@
         <f>A132+1</f>
         <v>665</v>
       </c>
-      <c r="B133" s="18" t="s">
-        <v>105</v>
+      <c r="B133" s="18">
+        <v>44012.512499999997</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -14623,7 +14617,7 @@
         <v>20</v>
       </c>
       <c r="M133" s="16" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="N133" s="16" t="s">
         <v>103</v>
@@ -14706,8 +14700,8 @@
       <c r="AO133">
         <v>0</v>
       </c>
-      <c r="AP133" t="s">
-        <v>107</v>
+      <c r="AP133">
+        <v>1</v>
       </c>
       <c r="AQ133" s="1">
         <f>52+17/60</f>
@@ -14729,6 +14723,444 @@
       </c>
       <c r="AV133" s="16" t="s">
         <v>29</v>
+      </c>
+      <c r="AW133" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX133" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <f>A133+1</f>
+        <v>666</v>
+      </c>
+      <c r="B134" s="18">
+        <v>44013.49722222222</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="F134" t="s">
+        <v>49</v>
+      </c>
+      <c r="G134" s="17">
+        <f>AVERAGE(91,92,94)</f>
+        <v>92.333333333333329</v>
+      </c>
+      <c r="H134" s="17">
+        <f>AVERAGE(76,75)</f>
+        <v>75.5</v>
+      </c>
+      <c r="I134" s="17">
+        <f>AVERAGE(58,59,56)</f>
+        <v>57.666666666666664</v>
+      </c>
+      <c r="J134" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="K134" s="17">
+        <f>AVERAGE(15,13,13)</f>
+        <v>13.666666666666666</v>
+      </c>
+      <c r="L134" s="17">
+        <v>25</v>
+      </c>
+      <c r="M134" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="N134" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="O134" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="P134" s="1">
+        <v>4.88</v>
+      </c>
+      <c r="Q134" s="17">
+        <v>1252</v>
+      </c>
+      <c r="R134" s="17">
+        <v>16054</v>
+      </c>
+      <c r="S134" s="17">
+        <f>R134-Q134</f>
+        <v>14802</v>
+      </c>
+      <c r="T134" s="1">
+        <f>(60+52)/60</f>
+        <v>1.8666666666666667</v>
+      </c>
+      <c r="U134" s="1">
+        <f>(60+58)/60</f>
+        <v>1.9666666666666666</v>
+      </c>
+      <c r="V134" s="1">
+        <f t="shared" si="85"/>
+        <v>9.9999999999999867E-2</v>
+      </c>
+      <c r="W134" s="1">
+        <f t="shared" ref="W134" si="115">P134/T134</f>
+        <v>2.6142857142857143</v>
+      </c>
+      <c r="X134">
+        <v>3</v>
+      </c>
+      <c r="Y134" s="1">
+        <f t="shared" ref="Y134" si="116">P134/X134</f>
+        <v>1.6266666666666667</v>
+      </c>
+      <c r="Z134" s="1">
+        <f>22+57/60</f>
+        <v>22.95</v>
+      </c>
+      <c r="AA134" s="17">
+        <v>469</v>
+      </c>
+      <c r="AB134" s="17">
+        <v>999</v>
+      </c>
+      <c r="AC134" s="17">
+        <v>116</v>
+      </c>
+      <c r="AD134" s="17">
+        <v>157</v>
+      </c>
+      <c r="AE134" s="1">
+        <f>24+43/60</f>
+        <v>24.716666666666665</v>
+      </c>
+      <c r="AF134" s="1">
+        <f>12+6/60</f>
+        <v>12.1</v>
+      </c>
+      <c r="AG134" s="1">
+        <f>22+54/60</f>
+        <v>22.9</v>
+      </c>
+      <c r="AH134" s="1">
+        <f>60/2.8</f>
+        <v>21.428571428571431</v>
+      </c>
+      <c r="AO134">
+        <v>2</v>
+      </c>
+      <c r="AP134">
+        <v>1</v>
+      </c>
+      <c r="AQ134" s="1">
+        <f>1+23/60</f>
+        <v>1.3833333333333333</v>
+      </c>
+      <c r="AR134" s="1">
+        <f>22+44/60</f>
+        <v>22.733333333333334</v>
+      </c>
+      <c r="AS134" s="1">
+        <f>27+52/60</f>
+        <v>27.866666666666667</v>
+      </c>
+      <c r="AT134" s="1">
+        <f>57+46/60</f>
+        <v>57.766666666666666</v>
+      </c>
+      <c r="AU134" s="1">
+        <f>2+12/60</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AV134" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW134" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX134" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <f t="shared" ref="A135:A136" si="117">A134+1</f>
+        <v>667</v>
+      </c>
+      <c r="B135" s="18">
+        <v>44014.55</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="F135" t="s">
+        <v>45</v>
+      </c>
+      <c r="G135" s="17">
+        <v>92</v>
+      </c>
+      <c r="H135" s="17">
+        <v>76</v>
+      </c>
+      <c r="I135" s="17">
+        <v>59</v>
+      </c>
+      <c r="J135" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="K135" s="17">
+        <v>10</v>
+      </c>
+      <c r="L135" s="17">
+        <v>0</v>
+      </c>
+      <c r="M135" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="N135" t="s">
+        <v>33</v>
+      </c>
+      <c r="O135" t="s">
+        <v>101</v>
+      </c>
+      <c r="P135" s="1">
+        <v>2.52</v>
+      </c>
+      <c r="T135" s="1">
+        <f>64/60</f>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="U135" s="1">
+        <f>64/60</f>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="V135" s="1">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="W135" s="1">
+        <f t="shared" ref="W135" si="118">P135/T135</f>
+        <v>2.3625000000000003</v>
+      </c>
+      <c r="X135">
+        <v>2</v>
+      </c>
+      <c r="Y135" s="1">
+        <f t="shared" ref="Y135" si="119">P135/X135</f>
+        <v>1.26</v>
+      </c>
+      <c r="Z135" s="1">
+        <f>25+28/60</f>
+        <v>25.466666666666665</v>
+      </c>
+      <c r="AA135" s="17">
+        <v>79</v>
+      </c>
+      <c r="AB135" s="17">
+        <v>277</v>
+      </c>
+      <c r="AC135" s="17">
+        <v>79</v>
+      </c>
+      <c r="AD135" s="17">
+        <v>110</v>
+      </c>
+      <c r="AE135" s="1">
+        <f>25+18/60</f>
+        <v>25.3</v>
+      </c>
+      <c r="AF135" s="1">
+        <f>24+59/60</f>
+        <v>24.983333333333334</v>
+      </c>
+      <c r="AG135" s="1">
+        <f>60/2.4</f>
+        <v>25</v>
+      </c>
+      <c r="AO135">
+        <v>0</v>
+      </c>
+      <c r="AP135">
+        <v>0</v>
+      </c>
+      <c r="AQ135" s="1">
+        <f>13+23/60</f>
+        <v>13.383333333333333</v>
+      </c>
+      <c r="AR135" s="1">
+        <f>23+15/60</f>
+        <v>23.25</v>
+      </c>
+      <c r="AS135" s="1">
+        <f>39/60</f>
+        <v>0.65</v>
+      </c>
+      <c r="AT135" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU135" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV135" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW135" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX135" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <f t="shared" si="117"/>
+        <v>668</v>
+      </c>
+      <c r="B136" s="18">
+        <v>44015.503472222219</v>
+      </c>
+      <c r="C136">
+        <v>1</v>
+      </c>
+      <c r="F136" t="s">
+        <v>31</v>
+      </c>
+      <c r="G136" s="17">
+        <f>AVERAGE(95,96)</f>
+        <v>95.5</v>
+      </c>
+      <c r="H136" s="17">
+        <f>AVERAGE(67,64)</f>
+        <v>65.5</v>
+      </c>
+      <c r="I136" s="17">
+        <f>AVERAGE(40,35)</f>
+        <v>37.5</v>
+      </c>
+      <c r="J136" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="K136" s="17">
+        <v>3</v>
+      </c>
+      <c r="L136" s="17">
+        <v>0</v>
+      </c>
+      <c r="M136" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="N136" t="s">
+        <v>103</v>
+      </c>
+      <c r="O136" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="P136" s="1">
+        <v>5.08</v>
+      </c>
+      <c r="Q136" s="17">
+        <v>995</v>
+      </c>
+      <c r="R136" s="17">
+        <v>16402</v>
+      </c>
+      <c r="S136" s="17">
+        <f>R136-Q136</f>
+        <v>15407</v>
+      </c>
+      <c r="T136" s="1">
+        <f>122/60</f>
+        <v>2.0333333333333332</v>
+      </c>
+      <c r="U136" s="1">
+        <f>122/60</f>
+        <v>2.0333333333333332</v>
+      </c>
+      <c r="V136" s="1">
+        <f t="shared" si="85"/>
+        <v>0</v>
+      </c>
+      <c r="W136" s="1">
+        <f t="shared" ref="W136" si="120">P136/T136</f>
+        <v>2.4983606557377049</v>
+      </c>
+      <c r="X136">
+        <v>4</v>
+      </c>
+      <c r="Y136" s="1">
+        <f t="shared" ref="Y136" si="121">P136/X136</f>
+        <v>1.27</v>
+      </c>
+      <c r="Z136" s="1">
+        <f>24+2/60</f>
+        <v>24.033333333333335</v>
+      </c>
+      <c r="AA136" s="17">
+        <v>62</v>
+      </c>
+      <c r="AB136" s="17">
+        <v>709</v>
+      </c>
+      <c r="AC136" s="17">
+        <v>97</v>
+      </c>
+      <c r="AD136" s="17">
+        <v>129</v>
+      </c>
+      <c r="AE136" s="1">
+        <f>23+25/60</f>
+        <v>23.416666666666668</v>
+      </c>
+      <c r="AF136" s="1">
+        <f>22+45/60</f>
+        <v>22.75</v>
+      </c>
+      <c r="AG136" s="1">
+        <f>28+21/60</f>
+        <v>28.35</v>
+      </c>
+      <c r="AH136" s="1">
+        <f>25+59/60</f>
+        <v>25.983333333333334</v>
+      </c>
+      <c r="AI136" s="1">
+        <f>19+52/60</f>
+        <v>19.866666666666667</v>
+      </c>
+      <c r="AJ136" s="1">
+        <f>60/2.8</f>
+        <v>21.428571428571431</v>
+      </c>
+      <c r="AO136">
+        <v>0</v>
+      </c>
+      <c r="AP136">
+        <v>0</v>
+      </c>
+      <c r="AQ136" s="1">
+        <f>16+9/60</f>
+        <v>16.149999999999999</v>
+      </c>
+      <c r="AR136" s="1">
+        <f>39+14/60</f>
+        <v>39.233333333333334</v>
+      </c>
+      <c r="AS136" s="1">
+        <f>27+38/60</f>
+        <v>27.633333333333333</v>
+      </c>
+      <c r="AT136" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU136" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV136" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW136" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX136" s="16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020-09-09-25 21:00 1. Changed name functions/compute_totals.R              to functions/compute_totals.R 2. Delete  tests/make_test_data.R 3. Added   tests/test__compute_totals.Rmd 4. Deleted teests/rest_compute_walk_history.R 5. Delete tests/.test__filter_by_days.R 6. Added todays walk to data/dys.xlsx
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="139">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -435,6 +435,9 @@
   <si>
     <t xml:space="preserve">Vandergriff Park – Highlands</t>
   </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
 </sst>
 </file>
 
@@ -642,15 +645,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB220"/>
+  <dimension ref="A1:BB221"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AI1" activeCellId="0" sqref="AI1"/>
-      <selection pane="bottomLeft" activeCell="AY220" activeCellId="0" sqref="AY220:BB220"/>
+      <selection pane="topLeft" activeCell="AG1" activeCellId="0" sqref="AG1"/>
+      <selection pane="bottomLeft" activeCell="AY221" activeCellId="0" sqref="AY221:BA221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.03"/>
@@ -674,7 +677,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="3" width="7.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="9.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="6.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="4.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="3" width="4.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="3" width="6.35"/>
@@ -26175,6 +26178,171 @@
         <v>0</v>
       </c>
     </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="n">
+        <f aca="false">A220+1</f>
+        <v>753</v>
+      </c>
+      <c r="B221" s="1" t="n">
+        <v>44099.5118055556</v>
+      </c>
+      <c r="C221" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F221" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G221" s="2" t="n">
+        <f aca="false">(73+76)/2</f>
+        <v>74.5</v>
+      </c>
+      <c r="H221" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="I221" s="2" t="n">
+        <f aca="false">(73+67)/2</f>
+        <v>70</v>
+      </c>
+      <c r="J221" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K221" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="L221" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M221" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="O221" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="P221" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q221" s="3" t="n">
+        <v>6.83</v>
+      </c>
+      <c r="R221" s="2" t="n">
+        <v>616</v>
+      </c>
+      <c r="S221" s="2" t="n">
+        <v>15219</v>
+      </c>
+      <c r="T221" s="2" t="n">
+        <f aca="false">S221-R221</f>
+        <v>14603</v>
+      </c>
+      <c r="U221" s="3" t="n">
+        <f aca="false">(60+58)/60</f>
+        <v>1.96666666666667</v>
+      </c>
+      <c r="V221" s="3" t="n">
+        <f aca="false">(120+23)/60</f>
+        <v>2.38333333333333</v>
+      </c>
+      <c r="W221" s="3" t="n">
+        <f aca="false">V221-U221</f>
+        <v>0.416666666666667</v>
+      </c>
+      <c r="X221" s="3" t="n">
+        <f aca="false">Q221/U221</f>
+        <v>3.4728813559322</v>
+      </c>
+      <c r="Y221" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z221" s="3" t="n">
+        <f aca="false">Q221/Y221</f>
+        <v>6.83</v>
+      </c>
+      <c r="AA221" s="3" t="n">
+        <f aca="false">17+16/60</f>
+        <v>17.2666666666667</v>
+      </c>
+      <c r="AB221" s="2" t="n">
+        <v>1752</v>
+      </c>
+      <c r="AC221" s="2" t="n">
+        <v>696</v>
+      </c>
+      <c r="AD221" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="AE221" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="AF221" s="3" t="n">
+        <f aca="false">15+46/60</f>
+        <v>15.7666666666667</v>
+      </c>
+      <c r="AG221" s="3" t="n">
+        <f aca="false">15+19/60</f>
+        <v>15.3166666666667</v>
+      </c>
+      <c r="AH221" s="3" t="n">
+        <f aca="false">15+29/60</f>
+        <v>15.4833333333333</v>
+      </c>
+      <c r="AI221" s="3" t="n">
+        <f aca="false">16+47/60</f>
+        <v>16.7833333333333</v>
+      </c>
+      <c r="AJ221" s="3" t="n">
+        <f aca="false">18+44/60</f>
+        <v>18.7333333333333</v>
+      </c>
+      <c r="AK221" s="3" t="n">
+        <f aca="false">18+33/60</f>
+        <v>18.55</v>
+      </c>
+      <c r="AL221" s="3" t="n">
+        <f aca="false">17+16/60</f>
+        <v>17.2666666666667</v>
+      </c>
+      <c r="AP221" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AQ221" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR221" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS221" s="4" t="n">
+        <f aca="false">60*U221-SUM(AT221:AX221)</f>
+        <v>29.65</v>
+      </c>
+      <c r="AT221" s="3" t="n">
+        <f aca="false">27+57/60</f>
+        <v>27.95</v>
+      </c>
+      <c r="AU221" s="3" t="n">
+        <f aca="false">37+56/60</f>
+        <v>37.9333333333333</v>
+      </c>
+      <c r="AV221" s="3" t="n">
+        <f aca="false">20+34/60</f>
+        <v>20.5666666666667</v>
+      </c>
+      <c r="AW221" s="3" t="n">
+        <f aca="false">1+54/60</f>
+        <v>1.9</v>
+      </c>
+      <c r="AX221" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY221" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ221" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA221" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add today's walk to data/days.xlsx
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="138">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -435,9 +435,6 @@
   <si>
     <t xml:space="preserve">Vandergriff Park – Highlands</t>
   </si>
-  <si>
-    <t xml:space="preserve">s</t>
-  </si>
 </sst>
 </file>
 
@@ -645,15 +642,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB221"/>
+  <dimension ref="A1:BB222"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AG1" activeCellId="0" sqref="AG1"/>
-      <selection pane="bottomLeft" activeCell="AY221" activeCellId="0" sqref="AY221:BA221"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A222" activeCellId="0" sqref="A222"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.03"/>
@@ -677,7 +674,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="3" width="7.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="6.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="4.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="3" width="4.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="3" width="6.35"/>
@@ -25934,7 +25931,7 @@
       </c>
       <c r="W219" s="3" t="n">
         <f aca="false">V219-U219</f>
-        <v>0.116666666666667</v>
+        <v>0.11666666666666</v>
       </c>
       <c r="X219" s="3" t="n">
         <f aca="false">Q219/U219</f>
@@ -26002,7 +25999,7 @@
       </c>
       <c r="AS219" s="4" t="n">
         <f aca="false">60*U219-SUM(AT219:AX219)</f>
-        <v>59.7</v>
+        <v>59.7000000000002</v>
       </c>
       <c r="AT219" s="3" t="n">
         <f aca="false">45+39/60</f>
@@ -26204,7 +26201,7 @@
         <v>70</v>
       </c>
       <c r="J221" s="2" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="K221" s="2" t="n">
         <v>10</v>
@@ -26340,6 +26337,172 @@
         <v>58</v>
       </c>
       <c r="BA221" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="n">
+        <f aca="false">A221+1</f>
+        <v>754</v>
+      </c>
+      <c r="B222" s="1" t="n">
+        <v>44100.5222222222</v>
+      </c>
+      <c r="C222" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F222" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G222" s="2" t="n">
+        <f aca="false">(84+86+87)/3</f>
+        <v>85.6666666666667</v>
+      </c>
+      <c r="H222" s="2" t="n">
+        <f aca="false">(69+69+66)/3</f>
+        <v>68</v>
+      </c>
+      <c r="I222" s="2" t="n">
+        <f aca="false">(67+57+49)/3</f>
+        <v>57.6666666666667</v>
+      </c>
+      <c r="J222" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K222" s="2" t="n">
+        <f aca="false">(12+16+15)/2</f>
+        <v>21.5</v>
+      </c>
+      <c r="L222" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="M222" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="N222" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O222" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="P222" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q222" s="3" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="R222" s="2" t="n">
+        <v>708</v>
+      </c>
+      <c r="S222" s="2" t="n">
+        <v>14498</v>
+      </c>
+      <c r="T222" s="2" t="n">
+        <f aca="false">S222-R222</f>
+        <v>13790</v>
+      </c>
+      <c r="U222" s="3" t="n">
+        <f aca="false">(60+84)/60</f>
+        <v>2.4</v>
+      </c>
+      <c r="V222" s="3" t="n">
+        <f aca="false">(120+29)/60</f>
+        <v>2.48333333333333</v>
+      </c>
+      <c r="W222" s="3" t="n">
+        <f aca="false">V222-U222</f>
+        <v>0.0833333333333335</v>
+      </c>
+      <c r="X222" s="3" t="n">
+        <f aca="false">Q222/U222</f>
+        <v>2.47916666666667</v>
+      </c>
+      <c r="Y222" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z222" s="3" t="n">
+        <f aca="false">Q222/Y222</f>
+        <v>5.95</v>
+      </c>
+      <c r="AA222" s="3" t="n">
+        <f aca="false">19+46/60</f>
+        <v>19.7666666666667</v>
+      </c>
+      <c r="AB222" s="2" t="n">
+        <v>1795</v>
+      </c>
+      <c r="AC222" s="2" t="n">
+        <v>716</v>
+      </c>
+      <c r="AD222" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="AE222" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="AF222" s="3" t="n">
+        <f aca="false">16+57/60</f>
+        <v>16.95</v>
+      </c>
+      <c r="AG222" s="3" t="n">
+        <f aca="false">17+46/60</f>
+        <v>17.7666666666667</v>
+      </c>
+      <c r="AH222" s="3" t="n">
+        <f aca="false">18+56/60</f>
+        <v>18.9333333333333</v>
+      </c>
+      <c r="AI222" s="3" t="n">
+        <f aca="false">22+51/60</f>
+        <v>22.85</v>
+      </c>
+      <c r="AJ222" s="3" t="n">
+        <f aca="false">22+51/60</f>
+        <v>22.85</v>
+      </c>
+      <c r="AK222" s="3" t="n">
+        <f aca="false">60/2.9</f>
+        <v>20.6896551724138</v>
+      </c>
+      <c r="AP222" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ222" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR222" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS222" s="4" t="n">
+        <f aca="false">60*U222-SUM(AT222:AX222)</f>
+        <v>32.3166666666667</v>
+      </c>
+      <c r="AT222" s="3" t="n">
+        <f aca="false">41+4/60</f>
+        <v>41.0666666666667</v>
+      </c>
+      <c r="AU222" s="3" t="n">
+        <f aca="false">56+8/60</f>
+        <v>56.1333333333333</v>
+      </c>
+      <c r="AV222" s="3" t="n">
+        <f aca="false">14+26/60</f>
+        <v>14.4333333333333</v>
+      </c>
+      <c r="AW222" s="3" t="n">
+        <f aca="false">3/60</f>
+        <v>0.05</v>
+      </c>
+      <c r="AX222" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY222" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ222" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA222" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2020-10-14 15:16 1. Update 0020_report_last_0007_days_walks.Rmd 2. Adde3d analysis/manual_imputation_of_walk.R 3. Delete data/compass.xlsx 4. Restored Stoval Park to active status in    data/routes.xlsx 5. Added    development/0010_qnqlysis_of_missing_steps.Rmd 6. Deleted functions/get_day_routes.R 7. Debugged get_day_routes.R 8. Added dubctuibs/plot_temp_and_dp.R 9. Added tests/0000_clean_directory.R 10. Added tests/ddelete_html.R 11. Deleted test__define_compas.Rmd
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="143">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -441,6 +441,15 @@
   <si>
     <t xml:space="preserve">Partly Cloudy / Windy </t>
   </si>
+  <si>
+    <t xml:space="preserve">Weather forecast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Green Oaks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farmin not charged</t>
+  </si>
 </sst>
 </file>
 
@@ -653,15 +662,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BC236"/>
+  <dimension ref="A1:BC240"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A236" activeCellId="0" sqref="A236"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="AM1" activeCellId="0" sqref="AM1"/>
+      <selection pane="bottomLeft" activeCell="BC241" activeCellId="0" sqref="BC241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.64"/>
@@ -27470,7 +27479,7 @@
         <v>17.1428571428571</v>
       </c>
       <c r="AP228" s="2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AQ228" s="0" t="n">
         <v>1</v>
@@ -28700,7 +28709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="n">
         <f aca="false">A235+1</f>
         <v>768</v>
@@ -28772,10 +28781,7 @@
         <f aca="false">V236-U236</f>
         <v>0.05</v>
       </c>
-      <c r="X236" s="3" t="n">
-        <f aca="false">Q236/U236</f>
-        <v>3.54285714285714</v>
-      </c>
+      <c r="X236" s="0"/>
       <c r="Y236" s="0" t="n">
         <v>1</v>
       </c>
@@ -28861,6 +28867,482 @@
       </c>
       <c r="BB236" s="0" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="n">
+        <f aca="false">A236+1</f>
+        <v>769</v>
+      </c>
+      <c r="B237" s="1" t="n">
+        <v>44115.4951388889</v>
+      </c>
+      <c r="C237" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D237" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="F237" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G237" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="H237" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="I237" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="J237" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K237" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="L237" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M237" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="N237" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="n">
+        <f aca="false">A237+1</f>
+        <v>770</v>
+      </c>
+      <c r="B238" s="1" t="n">
+        <v>44116.4597222222</v>
+      </c>
+      <c r="C238" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F238" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G238" s="2" t="n">
+        <f aca="false">(75+79)/2</f>
+        <v>77</v>
+      </c>
+      <c r="H238" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="I238" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="J238" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K238" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="L238" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="M238" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="N238" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O238" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="P238" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q238" s="3" t="n">
+        <v>6.85</v>
+      </c>
+      <c r="R238" s="2" t="n">
+        <v>860</v>
+      </c>
+      <c r="S238" s="2" t="n">
+        <f aca="false">T238+R238</f>
+        <v>15780</v>
+      </c>
+      <c r="T238" s="2" t="n">
+        <v>14920</v>
+      </c>
+      <c r="U238" s="3" t="n">
+        <f aca="false">(120+3)/60</f>
+        <v>2.05</v>
+      </c>
+      <c r="V238" s="3" t="n">
+        <f aca="false">(120+16)/60</f>
+        <v>2.26666666666667</v>
+      </c>
+      <c r="W238" s="3" t="n">
+        <f aca="false">V238-U238</f>
+        <v>0.216666666666667</v>
+      </c>
+      <c r="X238" s="3" t="n">
+        <f aca="false">Q236/U236</f>
+        <v>3.54285714285714</v>
+      </c>
+      <c r="Y238" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z238" s="3" t="n">
+        <f aca="false">Q238/Y238</f>
+        <v>6.85</v>
+      </c>
+      <c r="AA238" s="3" t="n">
+        <f aca="false">17+56/60</f>
+        <v>17.9333333333333</v>
+      </c>
+      <c r="AB238" s="2" t="n">
+        <v>292</v>
+      </c>
+      <c r="AC238" s="2" t="n">
+        <v>555</v>
+      </c>
+      <c r="AD238" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="AE238" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="AF238" s="3" t="n">
+        <f aca="false">16+52/60</f>
+        <v>16.8666666666667</v>
+      </c>
+      <c r="AG238" s="3" t="n">
+        <f aca="false">17+31/60</f>
+        <v>17.5166666666667</v>
+      </c>
+      <c r="AH238" s="3" t="n">
+        <f aca="false">17+54/60</f>
+        <v>17.9</v>
+      </c>
+      <c r="AI238" s="3" t="n">
+        <f aca="false">18+51/60</f>
+        <v>18.85</v>
+      </c>
+      <c r="AJ238" s="3" t="n">
+        <f aca="false">18+14/60</f>
+        <v>18.2333333333333</v>
+      </c>
+      <c r="AK238" s="3" t="n">
+        <f aca="false">17+54/60</f>
+        <v>17.9</v>
+      </c>
+      <c r="AL238" s="3" t="n">
+        <f aca="false">60/3.3</f>
+        <v>18.1818181818182</v>
+      </c>
+      <c r="AM238" s="0"/>
+      <c r="AP238" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="AQ238" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR238" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS238" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT238" s="4" t="n">
+        <f aca="false">60*U238-SUM(AU238:AY238)</f>
+        <v>116.433333333333</v>
+      </c>
+      <c r="AU238" s="3" t="n">
+        <f aca="false">6+18/60</f>
+        <v>6.3</v>
+      </c>
+      <c r="AV238" s="3" t="n">
+        <f aca="false">16/60</f>
+        <v>0.266666666666667</v>
+      </c>
+      <c r="AW238" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX238" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY238" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ238" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA238" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB238" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="n">
+        <v>771</v>
+      </c>
+      <c r="B239" s="1" t="n">
+        <v>44117.5930555556</v>
+      </c>
+      <c r="C239" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F239" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G239" s="2" t="n">
+        <f aca="false">(77+81)/2</f>
+        <v>79</v>
+      </c>
+      <c r="H239" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="I239" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="J239" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K239" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L239" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M239" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="N239" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O239" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="P239" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q239" s="3" t="n">
+        <v>7.71</v>
+      </c>
+      <c r="R239" s="2" t="n">
+        <v>500</v>
+      </c>
+      <c r="S239" s="2" t="n">
+        <v>17039</v>
+      </c>
+      <c r="T239" s="2" t="n">
+        <f aca="false">S239-R239</f>
+        <v>16539</v>
+      </c>
+      <c r="U239" s="3" t="n">
+        <f aca="false">(120+6)/60</f>
+        <v>2.1</v>
+      </c>
+      <c r="V239" s="3" t="n">
+        <f aca="false">(120+15)/60</f>
+        <v>2.25</v>
+      </c>
+      <c r="W239" s="3" t="n">
+        <f aca="false">V239-U239</f>
+        <v>0.15</v>
+      </c>
+      <c r="X239" s="3" t="n">
+        <f aca="false">Q239/U239</f>
+        <v>3.67142857142857</v>
+      </c>
+      <c r="Y239" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z239" s="3" t="n">
+        <f aca="false">Q239/Y239</f>
+        <v>7.71</v>
+      </c>
+      <c r="AA239" s="3" t="n">
+        <f aca="false">16+24/60</f>
+        <v>16.4</v>
+      </c>
+      <c r="AB239" s="2" t="n">
+        <v>1037</v>
+      </c>
+      <c r="AC239" s="2" t="n">
+        <v>820</v>
+      </c>
+      <c r="AD239" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="AE239" s="0" t="n">
+        <v>141</v>
+      </c>
+      <c r="AF239" s="3" t="n">
+        <f aca="false">16+31/60</f>
+        <v>16.5166666666667</v>
+      </c>
+      <c r="AG239" s="3" t="n">
+        <f aca="false">15+58/60</f>
+        <v>15.9666666666667</v>
+      </c>
+      <c r="AH239" s="3" t="n">
+        <f aca="false">16+7/60</f>
+        <v>16.1166666666667</v>
+      </c>
+      <c r="AI239" s="3" t="n">
+        <f aca="false">16+38/60</f>
+        <v>16.6333333333333</v>
+      </c>
+      <c r="AJ239" s="3" t="n">
+        <f aca="false">16+26/60</f>
+        <v>16.4333333333333</v>
+      </c>
+      <c r="AK239" s="3" t="n">
+        <f aca="false">15+54/60</f>
+        <v>15.9</v>
+      </c>
+      <c r="AL239" s="3" t="n">
+        <f aca="false">60/3.7</f>
+        <v>16.2162162162162</v>
+      </c>
+      <c r="AP239" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="AQ239" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR239" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS239" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT239" s="4" t="n">
+        <f aca="false">60*U239-SUM(AU239:AY239)</f>
+        <v>-0.450000000000003</v>
+      </c>
+      <c r="AU239" s="3" t="n">
+        <f aca="false">4+41/60</f>
+        <v>4.68333333333333</v>
+      </c>
+      <c r="AV239" s="3" t="n">
+        <f aca="false">26+32/60</f>
+        <v>26.5333333333333</v>
+      </c>
+      <c r="AW239" s="3" t="n">
+        <f aca="false">(95+14/60)</f>
+        <v>95.2333333333333</v>
+      </c>
+      <c r="AX239" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY239" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ239" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA239" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB239" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B240" s="1" t="n">
+        <v>44118.4534722222</v>
+      </c>
+      <c r="C240" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F240" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G240" s="2" t="n">
+        <f aca="false">79+11/60*(83-79)</f>
+        <v>79.7333333333333</v>
+      </c>
+      <c r="H240" s="2" t="n">
+        <f aca="false">60+11/60*(64-60)</f>
+        <v>60.7333333333333</v>
+      </c>
+      <c r="I240" s="2" t="n">
+        <f aca="false">56+11/60+(60-63)</f>
+        <v>53.1833333333333</v>
+      </c>
+      <c r="J240" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K240" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="L240" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="M240" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="N240" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O240" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="P240" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q240" s="3" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="T240" s="2" t="n">
+        <v>9478</v>
+      </c>
+      <c r="U240" s="3" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="X240" s="3" t="n">
+        <f aca="false">Q240/U240</f>
+        <v>3.78378378378378</v>
+      </c>
+      <c r="Y240" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z240" s="3" t="n">
+        <f aca="false">Q240/Y240</f>
+        <v>1.05</v>
+      </c>
+      <c r="AA240" s="3" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="AB240" s="2" t="n">
+        <v>98.5</v>
+      </c>
+      <c r="AC240" s="2" t="n">
+        <v>552</v>
+      </c>
+      <c r="AP240" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ240" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR240" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS240" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ240" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA240" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB240" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC240" s="0" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020-05007 18:54 Catchung up on missed data
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2581" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2603" uniqueCount="171">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -530,7 +530,10 @@
     <t xml:space="preserve">Low Power</t>
   </si>
   <si>
-    <t xml:space="preserve">Rosey Walk</t>
+    <t xml:space="preserve">Rosie Walk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical</t>
   </si>
 </sst>
 </file>
@@ -771,12 +774,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ442"/>
+  <dimension ref="A1:AMJ443"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A424" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B:B"/>
+      <selection pane="bottomLeft" activeCell="M443" activeCellId="0" sqref="M443"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -49719,7 +49722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="387" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="1" t="n">
         <f aca="false">A386+1</f>
         <v>921</v>
@@ -49761,38 +49764,41 @@
       <c r="O387" s="3" t="s">
         <v>156</v>
       </c>
+      <c r="P387" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="Q387" s="7" t="n">
-        <v>4.66</v>
+        <v>4.5</v>
       </c>
       <c r="R387" s="5" t="n">
-        <v>11638</v>
+        <v>10027</v>
       </c>
       <c r="S387" s="7" t="n">
         <f aca="false">79/60</f>
         <v>1.31666666666667</v>
       </c>
       <c r="T387" s="7" t="n">
-        <f aca="false">96/60</f>
-        <v>1.6</v>
+        <f aca="false">88/60</f>
+        <v>1.46666666666667</v>
       </c>
       <c r="U387" s="7" t="n">
         <f aca="false">T387-S387</f>
-        <v>0.283333333333333</v>
+        <v>0.149999999999997</v>
       </c>
       <c r="V387" s="7" t="n">
         <f aca="false">Q387/S387</f>
-        <v>3.53924050632911</v>
+        <v>3.41772151898733</v>
       </c>
       <c r="W387" s="3" t="n">
         <v>1</v>
       </c>
       <c r="X387" s="7" t="n">
         <f aca="false">Q387/1</f>
-        <v>4.66</v>
+        <v>4.5</v>
       </c>
       <c r="Y387" s="7" t="n">
-        <f aca="false">17+1/60</f>
-        <v>17.0166666666667</v>
+        <f aca="false">17+24/60</f>
+        <v>17.4</v>
       </c>
       <c r="Z387" s="5" t="n">
         <v>43</v>
@@ -49811,39 +49817,40 @@
         <v>16.2166666666667</v>
       </c>
       <c r="AE387" s="7" t="n">
-        <f aca="false">15+58/60</f>
-        <v>15.9666666666667</v>
+        <f aca="false">17+2/60</f>
+        <v>17.0333333333333</v>
       </c>
       <c r="AF387" s="8" t="n">
-        <f aca="false">18+39/60</f>
-        <v>18.65</v>
+        <f aca="false">17+13/60</f>
+        <v>17.2166666666667</v>
       </c>
       <c r="AG387" s="7" t="n">
-        <f aca="false">16+40/60</f>
-        <v>16.6666666666667</v>
+        <f aca="false">18+35/60</f>
+        <v>18.5833333333333</v>
       </c>
       <c r="AH387" s="7" t="n">
-        <f aca="false">(11+46/60)/0.66</f>
-        <v>17.8282828282828</v>
+        <f aca="false">60/3.4</f>
+        <v>17.6470588235294</v>
       </c>
       <c r="AQ387" s="9" t="n">
         <f aca="false">60*S387-AR387-AS387-AT387-AU387-AV387</f>
-        <v>-0.00333333333317221</v>
+        <v>1.51666666666686</v>
       </c>
       <c r="AR387" s="7" t="n">
-        <f aca="false">5+25/60</f>
-        <v>5.41666666666667</v>
+        <f aca="false">1+29/60</f>
+        <v>1.48333333333333</v>
       </c>
       <c r="AS387" s="7" t="n">
-        <f aca="false">23+34/60</f>
-        <v>23.5666666666667</v>
+        <f aca="false">10+38/60</f>
+        <v>10.6333333333333</v>
       </c>
       <c r="AT387" s="7" t="n">
-        <f aca="false">47+36/60</f>
-        <v>47.6</v>
+        <f aca="false">65+6/60</f>
+        <v>65.1</v>
       </c>
       <c r="AU387" s="7" t="n">
-        <v>2.42</v>
+        <f aca="false">16/60</f>
+        <v>0.266666666666667</v>
       </c>
       <c r="AV387" s="7" t="n">
         <v>0</v>
@@ -49870,6 +49877,9 @@
       <c r="C388" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D388" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="F388" s="4" t="s">
         <v>59</v>
       </c>
@@ -49894,6 +49904,13 @@
       <c r="M388" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="N388" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O388" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="R388" s="0"/>
     </row>
     <row r="389" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="1" t="n">
@@ -49904,6 +49921,138 @@
         <f aca="false">B388+1</f>
         <v>44269</v>
       </c>
+      <c r="C389" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F389" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G389" s="5" t="n">
+        <v>59</v>
+      </c>
+      <c r="H389" s="5" t="n">
+        <v>46</v>
+      </c>
+      <c r="I389" s="5" t="n">
+        <v>52</v>
+      </c>
+      <c r="J389" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K389" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="L389" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M389" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N389" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O389" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="P389" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q389" s="7" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="R389" s="5" t="n">
+        <v>12496</v>
+      </c>
+      <c r="S389" s="18" t="n">
+        <f aca="false">76/60</f>
+        <v>1.26666666666667</v>
+      </c>
+      <c r="T389" s="7" t="n">
+        <f aca="false">78/60</f>
+        <v>1.3</v>
+      </c>
+      <c r="U389" s="7" t="n">
+        <f aca="false">T389-S389</f>
+        <v>0.0333333333333334</v>
+      </c>
+      <c r="V389" s="7" t="n">
+        <f aca="false">Q389/S389</f>
+        <v>3.70263157894737</v>
+      </c>
+      <c r="W389" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="X389" s="7" t="n">
+        <f aca="false">Q389/1</f>
+        <v>4.69</v>
+      </c>
+      <c r="Y389" s="7" t="n">
+        <f aca="false">16+18/60</f>
+        <v>16.3</v>
+      </c>
+      <c r="Z389" s="5" t="n">
+        <v>102</v>
+      </c>
+      <c r="AA389" s="5" t="n">
+        <v>516</v>
+      </c>
+      <c r="AB389" s="5" t="n">
+        <v>128</v>
+      </c>
+      <c r="AC389" s="3" t="n">
+        <v>146</v>
+      </c>
+      <c r="AD389" s="7" t="n">
+        <f aca="false">16+6/60</f>
+        <v>16.1</v>
+      </c>
+      <c r="AE389" s="7" t="n">
+        <f aca="false">16</f>
+        <v>16</v>
+      </c>
+      <c r="AF389" s="8" t="n">
+        <f aca="false">16+30/60</f>
+        <v>16.5</v>
+      </c>
+      <c r="AG389" s="7" t="n">
+        <f aca="false">16+29/60</f>
+        <v>16.4833333333333</v>
+      </c>
+      <c r="AH389" s="7" t="n">
+        <f aca="false">60/3.6</f>
+        <v>16.6666666666667</v>
+      </c>
+      <c r="AQ389" s="9" t="n">
+        <f aca="false">60*S389-AR389-AS389-AT389-AU389-AV389</f>
+        <v>-0.00333333333333008</v>
+      </c>
+      <c r="AR389" s="7" t="n">
+        <f aca="false">4+2/60</f>
+        <v>4.03333333333333</v>
+      </c>
+      <c r="AS389" s="7" t="n">
+        <f aca="false">17+38/60</f>
+        <v>17.6333333333333</v>
+      </c>
+      <c r="AT389" s="7" t="n">
+        <f aca="false">52+31/60</f>
+        <v>52.5166666666667</v>
+      </c>
+      <c r="AU389" s="7" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="AV389" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW389" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AX389" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY389" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="390" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="1" t="n">
@@ -50414,8 +50563,20 @@
         <f aca="false">B439+1</f>
         <v>44320</v>
       </c>
+      <c r="C440" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX440" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY440" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ440" s="3" t="s">
+        <v>168</v>
+      </c>
     </row>
-    <row r="441" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="441" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="1" t="n">
         <f aca="false">A440+1</f>
         <v>975</v>
@@ -50425,22 +50586,150 @@
         <v>44321</v>
       </c>
       <c r="C441" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW441" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F441" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G441" s="5" t="n">
+        <v>68</v>
+      </c>
+      <c r="H441" s="5" t="n">
+        <v>56</v>
+      </c>
+      <c r="I441" s="5" t="n">
+        <v>65</v>
+      </c>
+      <c r="J441" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K441" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="L441" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M441" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N441" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="P441" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q441" s="7" t="n">
+        <v>5.17</v>
+      </c>
+      <c r="R441" s="5" t="n">
+        <v>14318</v>
+      </c>
+      <c r="S441" s="7" t="n">
+        <f aca="false">(60+46)/60</f>
+        <v>1.76666666666667</v>
+      </c>
+      <c r="T441" s="7" t="n">
+        <f aca="false">128/60</f>
+        <v>2.13333333333333</v>
+      </c>
+      <c r="U441" s="7" t="n">
+        <f aca="false">T441-S441</f>
+        <v>0.366666666666667</v>
+      </c>
+      <c r="V441" s="7" t="n">
+        <f aca="false">Q441/S441</f>
+        <v>2.92641509433962</v>
+      </c>
+      <c r="W441" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="X441" s="7" t="n">
+        <f aca="false">Q441/1</f>
+        <v>5.17</v>
+      </c>
+      <c r="Y441" s="7" t="n">
+        <f aca="false">20+32/60</f>
+        <v>20.5333333333333</v>
+      </c>
+      <c r="Z441" s="5" t="n">
+        <f aca="false">596-493</f>
+        <v>103</v>
+      </c>
+      <c r="AA441" s="5" t="n">
+        <v>579</v>
+      </c>
+      <c r="AB441" s="5" t="n">
+        <v>106</v>
+      </c>
+      <c r="AC441" s="3" t="n">
+        <v>132</v>
+      </c>
+      <c r="AD441" s="7" t="n">
+        <f aca="false">18+32/60</f>
+        <v>18.5333333333333</v>
+      </c>
+      <c r="AE441" s="7" t="n">
+        <f aca="false">20+47/60</f>
+        <v>20.7833333333333</v>
+      </c>
+      <c r="AF441" s="8" t="n">
+        <f aca="false">22+4/60</f>
+        <v>22.0666666666667</v>
+      </c>
+      <c r="AG441" s="7" t="n">
+        <f aca="false">20+49/60</f>
+        <v>20.8166666666667</v>
+      </c>
+      <c r="AH441" s="7" t="n">
+        <f aca="false">20+5/60</f>
+        <v>20.0833333333333</v>
+      </c>
+      <c r="AI441" s="7" t="n">
+        <f aca="false">60/2.9</f>
+        <v>20.6896551724138</v>
+      </c>
+      <c r="AN441" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO441" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP441" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ441" s="9" t="n">
+        <f aca="false">60*S441-SUM(AR441:AV441)</f>
+        <v>6.23333333333335</v>
+      </c>
+      <c r="AR441" s="7" t="n">
+        <f aca="false">43+41/60</f>
+        <v>43.6833333333333</v>
+      </c>
+      <c r="AS441" s="7" t="n">
+        <f aca="false">54+25/60</f>
+        <v>54.4166666666667</v>
+      </c>
+      <c r="AT441" s="7" t="n">
+        <f aca="false">1+40/60</f>
+        <v>1.66666666666667</v>
+      </c>
+      <c r="AU441" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV441" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW441" s="9" t="s">
         <v>57</v>
       </c>
       <c r="AX441" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AY441" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ441" s="3" t="s">
-        <v>168</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="442" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="442" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="1" t="n">
         <f aca="false">A441+1</f>
         <v>976</v>
@@ -50453,13 +50742,13 @@
         <v>1</v>
       </c>
       <c r="F442" s="4" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="G442" s="5" t="n">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="H442" s="5" t="n">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I442" s="5" t="n">
         <v>65</v>
@@ -50483,77 +50772,76 @@
         <v>169</v>
       </c>
       <c r="Q442" s="7" t="n">
-        <v>5.17</v>
+        <v>5.48</v>
       </c>
       <c r="R442" s="5" t="n">
-        <v>14318</v>
+        <v>15148</v>
       </c>
       <c r="S442" s="7" t="n">
-        <f aca="false">(60+46)/60</f>
-        <v>1.76666666666667</v>
+        <f aca="false">(120+3)/60</f>
+        <v>2.05</v>
       </c>
       <c r="T442" s="7" t="n">
-        <f aca="false">128/60</f>
-        <v>2.13333333333333</v>
+        <f aca="false">150/60</f>
+        <v>2.5</v>
       </c>
       <c r="U442" s="7" t="n">
         <f aca="false">T442-S442</f>
-        <v>0.366666666666667</v>
+        <v>0.45</v>
       </c>
       <c r="V442" s="7" t="n">
         <f aca="false">Q442/S442</f>
-        <v>2.92641509433962</v>
+        <v>2.67317073170732</v>
       </c>
       <c r="W442" s="3" t="n">
         <v>1</v>
       </c>
       <c r="X442" s="7" t="n">
         <f aca="false">Q442/1</f>
-        <v>5.17</v>
+        <v>5.48</v>
       </c>
       <c r="Y442" s="7" t="n">
-        <f aca="false">20+32/60</f>
-        <v>20.5333333333333</v>
+        <f aca="false">22+31/60</f>
+        <v>22.5166666666667</v>
       </c>
       <c r="Z442" s="5" t="n">
-        <f aca="false">596-493</f>
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="AA442" s="5" t="n">
-        <v>579</v>
+        <v>632</v>
       </c>
       <c r="AB442" s="5" t="n">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="AC442" s="3" t="n">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="AD442" s="7" t="n">
-        <f aca="false">18+32/60</f>
-        <v>18.5333333333333</v>
+        <f aca="false">19+35/60</f>
+        <v>19.5833333333333</v>
       </c>
       <c r="AE442" s="7" t="n">
-        <f aca="false">20+47/60</f>
-        <v>20.7833333333333</v>
+        <f aca="false">21+27/60</f>
+        <v>21.45</v>
       </c>
       <c r="AF442" s="8" t="n">
-        <f aca="false">22+4/60</f>
-        <v>22.0666666666667</v>
+        <f aca="false">27+2/60</f>
+        <v>27.0333333333333</v>
       </c>
       <c r="AG442" s="7" t="n">
-        <f aca="false">20+49/60</f>
-        <v>20.8166666666667</v>
+        <f aca="false">22+33/60</f>
+        <v>22.55</v>
       </c>
       <c r="AH442" s="7" t="n">
-        <f aca="false">20+5/60</f>
-        <v>20.0833333333333</v>
+        <f aca="false">22+57/60</f>
+        <v>22.95</v>
       </c>
       <c r="AI442" s="7" t="n">
-        <f aca="false">60/2.9</f>
-        <v>20.6896551724138</v>
+        <f aca="false">60/2.7</f>
+        <v>22.2222222222222</v>
       </c>
       <c r="AN442" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AO442" s="3" t="n">
         <v>0</v>
@@ -50563,22 +50851,23 @@
       </c>
       <c r="AQ442" s="9" t="n">
         <f aca="false">60*S442-SUM(AR442:AV442)</f>
-        <v>6.23333333333335</v>
+        <v>0.983333333333334</v>
       </c>
       <c r="AR442" s="7" t="n">
-        <f aca="false">43+41/60</f>
-        <v>43.6833333333333</v>
+        <f aca="false">15+53/60</f>
+        <v>15.8833333333333</v>
       </c>
       <c r="AS442" s="7" t="n">
-        <f aca="false">54+25/60</f>
-        <v>54.4166666666667</v>
+        <f aca="false">75+28/60</f>
+        <v>75.4666666666667</v>
       </c>
       <c r="AT442" s="7" t="n">
-        <f aca="false">1+40/60</f>
-        <v>1.66666666666667</v>
+        <f aca="false">29+19/60</f>
+        <v>29.3166666666667</v>
       </c>
       <c r="AU442" s="7" t="n">
-        <v>0</v>
+        <f aca="false">1+21/60</f>
+        <v>1.35</v>
       </c>
       <c r="AV442" s="7" t="n">
         <v>0</v>
@@ -50591,6 +50880,46 @@
       </c>
       <c r="AY442" s="3" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="1" t="n">
+        <f aca="false">A442+1</f>
+        <v>977</v>
+      </c>
+      <c r="B443" s="2" t="n">
+        <f aca="false">B442+1</f>
+        <v>44323</v>
+      </c>
+      <c r="C443" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D443" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F443" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G443" s="5" t="n">
+        <v>78</v>
+      </c>
+      <c r="H443" s="5" t="n">
+        <v>55</v>
+      </c>
+      <c r="I443" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="J443" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K443" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="L443" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="M443" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added days to data/days.xlsx
</commit_message>
<xml_diff>
--- a/data/days.xlsx
+++ b/data/days.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2708" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2742" uniqueCount="174">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -527,7 +527,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Calm</t>
+    <t xml:space="preserve">Lost data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Failure</t>
   </si>
   <si>
     <t xml:space="preserve">Rosie – Stovall to Kane Parks</t>
@@ -780,12 +783,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ448"/>
+  <dimension ref="A1:AMJ450"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A394" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D449" activeCellId="0" sqref="D449"/>
+      <selection pane="bottomLeft" activeCell="A402" activeCellId="0" sqref="A402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -50942,7 +50945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="400" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="1" t="n">
         <f aca="false">A399+1</f>
         <v>934</v>
@@ -50951,8 +50954,38 @@
         <f aca="false">B399+1</f>
         <v>44280</v>
       </c>
+      <c r="C400" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D400" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F400" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G400" s="5" t="n">
+        <v>59</v>
+      </c>
+      <c r="H400" s="5" t="n">
+        <v>49</v>
+      </c>
+      <c r="I400" s="5" t="n">
+        <v>69</v>
+      </c>
+      <c r="J400" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K400" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="L400" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M400" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="401" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="401" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="n">
         <f aca="false">A400+1</f>
         <v>935</v>
@@ -50961,8 +50994,56 @@
         <f aca="false">B400+1</f>
         <v>44281</v>
       </c>
+      <c r="C401" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D401" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F401" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G401" s="5" t="n">
+        <v>73</v>
+      </c>
+      <c r="H401" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="I401" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="J401" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="K401" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="L401" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M401" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N401" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O401" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AW401" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AX401" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY401" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ401" s="3" t="s">
+        <v>169</v>
+      </c>
     </row>
-    <row r="402" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="402" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="1" t="n">
         <f aca="false">A401+1</f>
         <v>936</v>
@@ -50971,8 +51052,161 @@
         <f aca="false">B401+1</f>
         <v>44282</v>
       </c>
+      <c r="C402" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F402" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G402" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="H402" s="5" t="n">
+        <v>59</v>
+      </c>
+      <c r="I402" s="5" t="n">
+        <v>57</v>
+      </c>
+      <c r="J402" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K402" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="L402" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="M402" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N402" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O402" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="P402" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q402" s="7" t="n">
+        <v>7.11</v>
+      </c>
+      <c r="R402" s="5" t="n">
+        <v>17221</v>
+      </c>
+      <c r="S402" s="7" t="n">
+        <f aca="false">125/60</f>
+        <v>2.08333333333333</v>
+      </c>
+      <c r="T402" s="7" t="n">
+        <f aca="false">(120+19)/60</f>
+        <v>2.31666666666667</v>
+      </c>
+      <c r="U402" s="7" t="n">
+        <f aca="false">T402-S402</f>
+        <v>0.233333333333333</v>
+      </c>
+      <c r="V402" s="7" t="n">
+        <f aca="false">Q402/S402</f>
+        <v>3.4128</v>
+      </c>
+      <c r="W402" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="X402" s="7" t="n">
+        <f aca="false">Q402/1</f>
+        <v>7.11</v>
+      </c>
+      <c r="Y402" s="7" t="n">
+        <f aca="false">17+37/60</f>
+        <v>17.6166666666667</v>
+      </c>
+      <c r="Z402" s="5" t="n">
+        <v>866</v>
+      </c>
+      <c r="AA402" s="5" t="n">
+        <v>831</v>
+      </c>
+      <c r="AB402" s="5" t="n">
+        <v>136</v>
+      </c>
+      <c r="AC402" s="3" t="n">
+        <v>157</v>
+      </c>
+      <c r="AD402" s="7" t="n">
+        <f aca="false">16+40/60</f>
+        <v>16.6666666666667</v>
+      </c>
+      <c r="AE402" s="7" t="n">
+        <f aca="false">16+16/60</f>
+        <v>16.2666666666667</v>
+      </c>
+      <c r="AF402" s="8" t="n">
+        <f aca="false">17+9/60</f>
+        <v>17.15</v>
+      </c>
+      <c r="AG402" s="7" t="n">
+        <f aca="false">18+7/60</f>
+        <v>18.1166666666667</v>
+      </c>
+      <c r="AH402" s="7" t="n">
+        <f aca="false">18+22/60</f>
+        <v>18.3666666666667</v>
+      </c>
+      <c r="AI402" s="7" t="n">
+        <f aca="false">18+22/60</f>
+        <v>18.3666666666667</v>
+      </c>
+      <c r="AJ402" s="7" t="n">
+        <f aca="false">17+26/60</f>
+        <v>17.4333333333333</v>
+      </c>
+      <c r="AK402" s="7" t="n">
+        <f aca="false">60/2.3</f>
+        <v>26.0869565217391</v>
+      </c>
+      <c r="AN402" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO402" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP402" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ402" s="9" t="n">
+        <f aca="false">60*S402-AR402-AS402-AT402-AU402-AV402</f>
+        <v>-0.00333333333332675</v>
+      </c>
+      <c r="AR402" s="7" t="n">
+        <f aca="false">2+27/60</f>
+        <v>2.45</v>
+      </c>
+      <c r="AS402" s="7" t="n">
+        <f aca="false">9+11/60</f>
+        <v>9.18333333333333</v>
+      </c>
+      <c r="AT402" s="7" t="n">
+        <f aca="false">86+45/60</f>
+        <v>86.75</v>
+      </c>
+      <c r="AU402" s="7" t="n">
+        <v>26.62</v>
+      </c>
+      <c r="AV402" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW402" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AX402" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY402" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row r="403" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="403" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="1" t="n">
         <f aca="false">A402+1</f>
         <v>937</v>
@@ -51311,8 +51545,38 @@
         <f aca="false">B435+1</f>
         <v>44316</v>
       </c>
+      <c r="C436" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D436" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F436" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G436" s="5" t="n">
+        <v>65</v>
+      </c>
+      <c r="H436" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="I436" s="5" t="n">
+        <v>84</v>
+      </c>
+      <c r="J436" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K436" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="L436" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M436" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="437" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="437" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="1" t="n">
         <f aca="false">A436+1</f>
         <v>971</v>
@@ -51340,7 +51604,7 @@
         <v>87</v>
       </c>
       <c r="J437" s="6" t="s">
-        <v>168</v>
+        <v>125</v>
       </c>
       <c r="K437" s="5" t="n">
         <v>0</v>
@@ -51395,7 +51659,7 @@
         <v>146</v>
       </c>
       <c r="P438" s="19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="Q438" s="7" t="n">
         <v>5.17</v>
@@ -51456,7 +51720,7 @@
         <v>1</v>
       </c>
       <c r="AZ439" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51502,7 +51766,7 @@
         <v>146</v>
       </c>
       <c r="P440" s="19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="Q440" s="7" t="n">
         <v>5.17</v>
@@ -51615,7 +51879,7 @@
         <v>1</v>
       </c>
       <c r="AZ440" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51702,7 +51966,7 @@
         <v>146</v>
       </c>
       <c r="P442" s="19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="Q442" s="7" t="n">
         <v>5.48</v>
@@ -51828,7 +52092,7 @@
         <v>0</v>
       </c>
       <c r="D443" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F443" s="4" t="s">
         <v>69</v>
@@ -51855,7 +52119,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="444" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="444" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="1" t="n">
         <f aca="false">A443+1</f>
         <v>978</v>
@@ -51898,7 +52162,7 @@
         <v>146</v>
       </c>
       <c r="P444" s="19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="Q444" s="7" t="n">
         <v>2.38</v>
@@ -51967,7 +52231,7 @@
       </c>
       <c r="AQ444" s="9" t="n">
         <f aca="false">60*S444-SUM(AR444:AV444)</f>
-        <v>4.3</v>
+        <v>4.29999999999993</v>
       </c>
       <c r="AR444" s="7" t="n">
         <f aca="false">30+40/60</f>
@@ -51982,6 +52246,9 @@
         <v>2.41666666666667</v>
       </c>
       <c r="AU444" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV444" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AW444" s="9" t="s">
@@ -52071,7 +52338,7 @@
         <v>0</v>
       </c>
       <c r="M446" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52148,6 +52415,168 @@
         <v>10</v>
       </c>
       <c r="L448" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M448" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="449" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A449" s="1" t="n">
+        <f aca="false">A448+1</f>
+        <v>983</v>
+      </c>
+      <c r="B449" s="2" t="n">
+        <f aca="false">B448+1</f>
+        <v>44329</v>
+      </c>
+      <c r="C449" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F449" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G449" s="5" t="n">
+        <v>69</v>
+      </c>
+      <c r="H449" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="I449" s="5" t="n">
+        <v>53</v>
+      </c>
+      <c r="J449" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K449" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="L449" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M449" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N449" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O449" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="P449" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q449" s="7" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="R449" s="5" t="n">
+        <v>15861</v>
+      </c>
+      <c r="S449" s="7" t="n">
+        <f aca="false">(60+55)/60</f>
+        <v>1.91666666666667</v>
+      </c>
+      <c r="T449" s="7" t="n">
+        <f aca="false">(120+24)/60</f>
+        <v>2.4</v>
+      </c>
+      <c r="U449" s="7" t="n">
+        <f aca="false">T449-S449</f>
+        <v>0.483333333333333</v>
+      </c>
+      <c r="V449" s="7" t="n">
+        <f aca="false">Q449/S449</f>
+        <v>3.39130434782609</v>
+      </c>
+      <c r="W449" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="X449" s="7" t="n">
+        <f aca="false">Q449/1</f>
+        <v>6.5</v>
+      </c>
+      <c r="Y449" s="7" t="n">
+        <f aca="false">17+38/60</f>
+        <v>17.6333333333333</v>
+      </c>
+      <c r="Z449" s="5" t="n">
+        <v>187</v>
+      </c>
+      <c r="AA449" s="5" t="n">
+        <v>688</v>
+      </c>
+      <c r="AB449" s="5" t="n">
+        <v>76</v>
+      </c>
+      <c r="AC449" s="3" t="n">
+        <v>109</v>
+      </c>
+      <c r="AD449" s="7" t="n">
+        <f aca="false">17+32/60</f>
+        <v>17.5333333333333</v>
+      </c>
+      <c r="AE449" s="7" t="n">
+        <f aca="false">17+9/60</f>
+        <v>17.15</v>
+      </c>
+      <c r="AF449" s="8" t="n">
+        <f aca="false">17+53/60</f>
+        <v>17.8833333333333</v>
+      </c>
+      <c r="AG449" s="7" t="n">
+        <f aca="false">17+32/60</f>
+        <v>17.5333333333333</v>
+      </c>
+      <c r="AH449" s="7" t="n">
+        <f aca="false">18+2/60</f>
+        <v>18.0333333333333</v>
+      </c>
+      <c r="AI449" s="7" t="n">
+        <f aca="false">17+54/60</f>
+        <v>17.9</v>
+      </c>
+      <c r="AJ449" s="7" t="n">
+        <f aca="false">60/3.4</f>
+        <v>17.6470588235294</v>
+      </c>
+    </row>
+    <row r="450" customFormat="false" ht="16.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AN450" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO450" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP450" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ450" s="9" t="n">
+        <f aca="false">60*S449-SUM(AR450:AV450)</f>
+        <v>114.766666666667</v>
+      </c>
+      <c r="AR450" s="7" t="n">
+        <f aca="false">14/60</f>
+        <v>0.233333333333333</v>
+      </c>
+      <c r="AS450" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT450" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU450" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV450" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW450" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AX450" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY450" s="3" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>